<commit_message>
Fix nuevo campo source
Se agrego un nuevo campo fuente
</commit_message>
<xml_diff>
--- a/src/assets/prototypes/disease.xlsx
+++ b/src/assets/prototypes/disease.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BDGSA\Desktop\PROTOTIPOS EXCEL\zPROTOS FINAL\PROTOTIPOS LIMPIOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BDGSA\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD87426-8908-4E55-AF5C-993A43C54939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7459671-9A67-4DD9-8E63-10301B7D2B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" tabRatio="819" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>name_en</t>
   </si>
@@ -51,147 +51,7 @@
     <t>description_fr</t>
   </si>
   <si>
-    <t>Hepatitis B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rotavirus </t>
-  </si>
-  <si>
-    <t>Neumococo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poliomielitis </t>
-  </si>
-  <si>
-    <t>Tuberculosis</t>
-  </si>
-  <si>
-    <t>La hepatitis B es una enfermedad grave que afecta al hígado y que es causada por el virus de la hepatitis B. La Hepatitis B puede provocar una enfermedad leve que dure algunas semanas, o puede llevar a una enfermedad grave de por vida.
-La infección por el virus de la hepatitis B puede ser aguda o crónica, pero se puede prevenir con la administración de la vacuna.</t>
-  </si>
-  <si>
-    <t>La tuberculosis (o TB, según su nombre abreviado) es una infección provocada por una bacteria llamada Mycobacterium tuberculosis (M. tuberculosis). Estas bacterias, o microbios, normalmente atacan los pulmones. Sin embargo, también pueden atacar otras partes del cuerpo, como los riñones, la columna vertebral o el cerebro.</t>
-  </si>
-  <si>
-    <t>La poliomielitis, o polio, es una enfermedad discapacitante causada por el virus poliomielítico que es potencialmente mortal. El virus puede infectar la médula espinal de las personas, lo cual causa parálisis (incapacidad de mover partes del cuerpo). La parálisis causada por la poliomielitis ocurre cuando el virus se reproduce dentro del sistema nervioso y lo ataca. La parálisis puede durar toda la vida, y también ser mortal.
-Con más frecuencia, enferma a los niños menores de 5 años.</t>
-  </si>
-  <si>
-    <t>El neumococo es una enfermedad causada por una bacteria que puede producir infecciones graves. Existen unas 100 variedades de neumococo, de los que solo algunos pueden producir infecciones en los seres humanos. Cuasando neumonía, o sea, una infección en el pulmón. 
-Los más vulnerables son los niños pequeños menores de 5 años y, en particular, los menores de 2 años.</t>
-  </si>
-  <si>
-    <t>Pneumococcus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tuberculosis </t>
-  </si>
-  <si>
-    <t>Hepatitis B is a serious disease that affects the liver and is caused by the hepatitis B virus. Hepatitis B can cause mild illness that lasts a few weeks, or it can lead to severe, life-long illness.
-Infection with the hepatitis B virus can be acute or chronic, but can be prevented with the administration of the vaccine.</t>
-  </si>
-  <si>
-    <t>Tuberculosis (or TB for short) is an infection caused by a bacterium called Mycobacterium tuberculosis (M. tuberculosis). These bacteria, or microbes, normally attack the lungs. However, they can also attack other parts of the body, such as the kidneys, spine, or brain.</t>
-  </si>
-  <si>
-    <t>Polio, or Poliomyelitis, is a disabling disease caused by the polio virus that is life threatening. The virus can infect people's spinal cord, causing paralysis (the inability to move parts of the body). The paralysis caused by polio occurs when the virus reproduces within the nervous system and attacks it. Paralysis can last a lifetime, and can also be fatal.
-Most often, it makes children younger than 5 sick.</t>
-  </si>
-  <si>
-    <t>Rotavirus is a disease that causes severe diarrhea and vomiting. It mainly affects babies and young children. Diarrhea and vomiting can lead to severe dehydration (loss of body fluids). If dehydration is not treated, it can be fatal.</t>
-  </si>
-  <si>
-    <t>Pneumococcus is a disease caused by bacteria that can lead to serious infections. There are about 100 varieties of pneumococcus, of which only some can cause infections in humans. Causing pneumonia, that is, an infection in the lung.
-The most vulnerable are young children under 5 years of age and, in particular, those under 2 years of age.</t>
-  </si>
-  <si>
-    <t>Rubeola</t>
-  </si>
-  <si>
-    <t>Sarampión</t>
-  </si>
-  <si>
-    <t>Poliomyelitis</t>
-  </si>
-  <si>
-    <t>Measles</t>
-  </si>
-  <si>
-    <t>Difteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tétanos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tosferina </t>
-  </si>
-  <si>
-    <t>Diphtheria</t>
-  </si>
-  <si>
-    <t>Tetanus</t>
-  </si>
-  <si>
-    <t>Es una enfermedad infecciosa aguda, provocada por un bacilo, que afecta a la nariz, la garganta y la laringe y produce fiebre y dificultad para respirar.
-Las bacterias de la difteria se propagan de persona a persona, por lo general a través de gotitas respiratorias, como al toser o estornudar. Antes de la introducción de vacunas, la difteria era una causa principal de muerte en la niñez en todo el mundo.</t>
-  </si>
-  <si>
-    <t>It is an acute infectious disease, caused by a bacillus, that affects the nose, throat and larynx and causes fever and shortness of breath.
-Diphtheria bacteria are spread from person to person, usually through respiratory droplets, such as coughing or sneezing. Before the introduction of vaccines, diphtheria was a leading cause of childhood death worldwide.</t>
-  </si>
-  <si>
-    <t>Es una enfermedad infecciosa, causada por un bacilo,que se produce por la infección de algunas heridas y que ataca al sistema nervioso.
-El tétanos se adquiere tras la infección de cortes o heridas por las esporas de la bacteria Clostridium tetani, y la mayoría de los casos aparecen a los 14 días de la infección.
-El tétanos es prevenible mediante la inmunización con vacunas que contienen toxoide tetánico. La mayoría de los casos de tétanos están relacionados con el parto y pueden afectar tanto a recién nacidos como a madres que no se hayan vacunado contra el Tétanos.</t>
-  </si>
-  <si>
-    <t>It is an infectious disease, caused by a bacillus, which is produced by the infection of some wounds and which attacks the nervous system.
-Tetanus is acquired after infection of cuts or wounds by spores of the bacterium Clostridium tetani, and most cases appear 14 days after infection.
-Tetanus is preventable by immunization with vaccines that contain tetanus toxoid. Most cases of tetanus are related to childbirth and can affect both newborns and mothers who have not been vaccinated against Tetanus.</t>
-  </si>
-  <si>
-    <t>La tosferina, también conocida como tos convulsa o pertussis, es una enfermedad muy contagiosa causada por un tipo de bacteria llamada Bordetella pertussis. Estas bacterias se adhieren a los cilios (pequeñas extensiones parecidas a vellos) que recubren parte del aparato respiratorio superior.
-La tosferina es una enfermedad muy contagiosa que solo se encuentra en los seres humanos. Se transmite de una persona a otra. Por lo general, las personas con tosferina les transmiten la enfermedad a los demás al toser o estornudar, o al pasar mucho tiempo en contacto cercano con ellos compartiendo el espacio donde respiran. Muchos bebés que contraen la tosferina se contagian de sus hermanos mayores, padres o las personas que los cuidan, quienes tal vez ni siquiera saben que tienen la enfermedad.</t>
-  </si>
-  <si>
-    <t>Whooping cough, also known as whooping cough or pertussis, is a highly contagious disease caused by a type of bacteria called Bordetella pertussis. These bacteria adhere to the cilia (small hair-like extensions) that line part of the upper respiratory tract.
-Whooping cough is a highly contagious disease found only in humans. It is transmitted from one person to another. People with whooping cough usually spread the disease to others by coughing or sneezing, or by spending a lot of time in close contact with them sharing their breathing space. Many babies who get whooping cough get it from older siblings, parents, or their caregivers, who may not even know they have the disease.</t>
-  </si>
-  <si>
-    <t>Es una enfermedad infecciosa y contagiosa, causada por un virus, que se caracteriza por la aparición de pequeñas manchas rojas en la piel, fiebre alta y síntomas catarrales; generalmente, se padece durante la infancia.
-El sarampión es altamente contagioso y puede causar complicaciones como diarrea, infecciones del oído, neumonía y encefalitis (inflamación del cerebro).</t>
-  </si>
-  <si>
-    <t>It is an infectious and contagious disease, caused by a virus, characterized by the appearance of small red spots on the skin, high fever and catarrhal symptoms; generally, it is suffered during childhood.
-Measles is highly contagious and can cause complications such as diarrhea, ear infections, pneumonia, and encephalitis (inflammation of the brain).</t>
-  </si>
-  <si>
-    <t>Parotiditis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parotiditis </t>
-  </si>
-  <si>
-    <t>La parotiditis es una enfermedad vírica que se caracteriza por fiebre e inflamación de una o más de las glándulas salivares, habitualmente de la parótida.
-La transmisión es por diseminación de gotitas de saliva o aerosoles o por contacto directo con la saliva de una persona infectada. Las personas asintomáticas o con infecciones atípicas pueden transmitir el virus.</t>
-  </si>
-  <si>
-    <t>Mumps is a viral disease characterized by fever and inflammation of one or more of the salivary glands, usually the parotid glands.
-Transmission is by the spread of saliva droplets or aerosols or by direct contact with the saliva of an infected person. Asymptomatic people or people with atypical infections can transmit the virus.</t>
-  </si>
-  <si>
-    <t>Rubella</t>
-  </si>
-  <si>
-    <t>La rubéola es una infección vírica aguda y contagiosa. Aunque el virus de la rubéola suele causar una enfermedad exantemática y febril leve en los niños y los adultos, la infección durante el embarazo, sobre todo en el primer trimestre, puede ser causa de aborto espontáneo, muerte fetal, muerte prenatal o malformaciones congénitas, que constituyen el llamado síndrome de rubéola congénita.
-El virus de la rubéola se transmite por gotículas en el aire, cuando las personas infectadas estornudan o tosen. No se dispone de un tratamiento específico para la rubéola, pero la enfermedad es prevenible con vacunas.</t>
-  </si>
-  <si>
-    <t>Rubella is an acute and contagious viral infection. Although the rubella virus usually causes a mild rash and fever in children and adults, infection during pregnancy, especially in the first trimester, can cause spontaneous abortion, fetal death, prenatal death, or congenital malformations. constituting the so-called congenital rubella syndrome.
-The rubella virus is transmitted by airborne droplets, when infected people sneeze or cough. There is no specific treatment for rubella, but the disease is preventable with vaccines.</t>
-  </si>
-  <si>
-    <t>El rotavirus es una enfermedad que causa diarrea y vómitos intensos. Afecta principalmente a bebés y niños pequeños. La diarrea y los vómitos pueden llevar a la deshidratación grave (pérdida de líquidos corporales). Si la deshidratación no se trata, puede ser mortal.</t>
+    <t>source</t>
   </si>
 </sst>
 </file>
@@ -270,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -278,19 +138,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -737,11 +588,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="B1:I23"/>
+  <dimension ref="B1:J17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -751,11 +602,11 @@
     <col min="6" max="6" width="49.25" customWidth="1"/>
     <col min="7" max="7" width="59.25" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
-    <col min="9" max="9" width="14.25" customWidth="1"/>
+    <col min="9" max="10" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="68.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="68.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -780,226 +631,154 @@
       <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" ht="141" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="J2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="2:9" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="2:9" ht="150" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="2:9" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="2:9" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-    </row>
-    <row r="8" spans="2:9" ht="153" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-    </row>
-    <row r="9" spans="2:9" ht="159" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-    </row>
-    <row r="10" spans="2:9" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-    </row>
-    <row r="11" spans="2:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-    </row>
-    <row r="12" spans="2:9" s="5" customFormat="1" ht="241.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-    </row>
-    <row r="13" spans="2:9" ht="297" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -1008,8 +787,9 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -1018,66 +798,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
+      <c r="J17" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>